<commit_message>
4.27 Finish Load System
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/StoryScript.xlsx
+++ b/Assets/StreamingAssets/StoryScript.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/renqi/TextAdvancedGame/Assets/StreamingAssets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFFA261E-734F-8640-B7D3-9D4FF411683C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A468C65E-CA6B-0E48-B367-D8685845FEE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15760" xr2:uid="{4FF494A4-B03B-D144-A30E-F081D1418406}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="87">
   <si>
     <t>Yao</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -365,7 +365,23 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>StoryScript</t>
+    <t>Q1C1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LastBGImage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LastBGM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LastX1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LastX2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -756,10 +772,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40E189AB-F231-6C46-8064-720ADE40C742}">
-  <dimension ref="A1:L47"/>
+  <dimension ref="A1:P47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView tabSelected="1" topLeftCell="B26" workbookViewId="0">
+      <selection activeCell="J49" sqref="J49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -776,10 +792,11 @@
     <col min="10" max="10" width="14.33203125" style="1" customWidth="1"/>
     <col min="11" max="11" width="9" style="1" customWidth="1"/>
     <col min="12" max="12" width="13.5" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="10.83203125" style="1"/>
+    <col min="13" max="13" width="18.33203125" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="17">
+    <row r="1" spans="1:16" ht="17">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -816,8 +833,20 @@
       <c r="L1" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="17">
+      <c r="M1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="17">
       <c r="B2" s="2" t="s">
         <v>71</v>
       </c>
@@ -831,65 +860,193 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="34">
+    <row r="3" spans="1:16" ht="34">
       <c r="B3" s="2" t="s">
         <v>30</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="34">
+      <c r="M3" s="1" t="str">
+        <f>IF(E2&lt;&gt;"",E2,M2)</f>
+        <v>Forest</v>
+      </c>
+      <c r="N3" s="1" t="str">
+        <f>IF(F2&lt;&gt;"",F2,N2)</f>
+        <v>Happy</v>
+      </c>
+      <c r="O3" s="1">
+        <f>IF(H2&lt;&gt;"",H2,O2)</f>
+        <v>0</v>
+      </c>
+      <c r="P3" s="1">
+        <f>IF(K2&lt;&gt;"",K2,P2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="34">
       <c r="B4" s="2" t="s">
         <v>31</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" ht="17">
+      <c r="M4" s="1" t="str">
+        <f t="shared" ref="M4:M46" si="0">IF(E3&lt;&gt;"",E3,M3)</f>
+        <v>Forest</v>
+      </c>
+      <c r="N4" s="1" t="str">
+        <f t="shared" ref="N4:N46" si="1">IF(F3&lt;&gt;"",F3,N3)</f>
+        <v>Happy</v>
+      </c>
+      <c r="O4" s="1">
+        <f t="shared" ref="O4:O46" si="2">IF(H3&lt;&gt;"",H3,O3)</f>
+        <v>0</v>
+      </c>
+      <c r="P4" s="1">
+        <f t="shared" ref="P4:P46" si="3">IF(K3&lt;&gt;"",K3,P3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="17">
       <c r="B5" s="2" t="s">
         <v>32</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" ht="17">
+      <c r="M5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Forest</v>
+      </c>
+      <c r="N5" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Happy</v>
+      </c>
+      <c r="O5" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P5" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="17">
       <c r="B6" s="2" t="s">
         <v>33</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" ht="34">
+      <c r="M6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Forest</v>
+      </c>
+      <c r="N6" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Happy</v>
+      </c>
+      <c r="O6" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P6" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="34">
       <c r="B7" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" ht="17">
+      <c r="M7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Forest</v>
+      </c>
+      <c r="N7" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Happy</v>
+      </c>
+      <c r="O7" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P7" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="17">
       <c r="B8" s="2" t="s">
         <v>35</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" ht="34">
+      <c r="M8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Forest</v>
+      </c>
+      <c r="N8" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Happy</v>
+      </c>
+      <c r="O8" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P8" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="34">
       <c r="B9" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" ht="34">
+      <c r="M9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Forest</v>
+      </c>
+      <c r="N9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Happy</v>
+      </c>
+      <c r="O9" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P9" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="34">
       <c r="B10" s="2" t="s">
         <v>37</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" ht="17">
+      <c r="M10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Forest</v>
+      </c>
+      <c r="N10" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Happy</v>
+      </c>
+      <c r="O10" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P10" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="17">
       <c r="A11" s="2" t="s">
         <v>0</v>
       </c>
@@ -902,16 +1059,48 @@
       <c r="D11" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" ht="34">
+      <c r="M11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Forest</v>
+      </c>
+      <c r="N11" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Happy</v>
+      </c>
+      <c r="O11" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P11" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="34">
       <c r="B12" s="2" t="s">
         <v>39</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" ht="17">
+      <c r="M12" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Forest</v>
+      </c>
+      <c r="N12" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Happy</v>
+      </c>
+      <c r="O12" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P12" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="17">
       <c r="A13" s="2" t="s">
         <v>0</v>
       </c>
@@ -924,8 +1113,24 @@
       <c r="D13" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" ht="17">
+      <c r="M13" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Forest</v>
+      </c>
+      <c r="N13" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Happy</v>
+      </c>
+      <c r="O13" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P13" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="17">
       <c r="B14" s="2" t="s">
         <v>41</v>
       </c>
@@ -935,8 +1140,24 @@
       <c r="D14" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" ht="17">
+      <c r="M14" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Forest</v>
+      </c>
+      <c r="N14" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Happy</v>
+      </c>
+      <c r="O14" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P14" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="17">
       <c r="A15" s="2" t="s">
         <v>1</v>
       </c>
@@ -958,8 +1179,24 @@
       <c r="I15" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" ht="17">
+      <c r="M15" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Forest</v>
+      </c>
+      <c r="N15" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Happy</v>
+      </c>
+      <c r="O15" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P15" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="17">
       <c r="A16" s="2" t="s">
         <v>0</v>
       </c>
@@ -972,8 +1209,27 @@
       <c r="D16" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" ht="17">
+      <c r="I16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M16" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Forest</v>
+      </c>
+      <c r="N16" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Happy</v>
+      </c>
+      <c r="O16" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P16" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" ht="17">
       <c r="A17" s="2" t="s">
         <v>1</v>
       </c>
@@ -995,8 +1251,24 @@
       <c r="I17" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" ht="34">
+      <c r="M17" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Forest</v>
+      </c>
+      <c r="N17" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Happy</v>
+      </c>
+      <c r="O17" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P17" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" ht="34">
       <c r="B18" s="2" t="s">
         <v>66</v>
       </c>
@@ -1006,8 +1278,27 @@
       <c r="G18" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" ht="17">
+      <c r="I18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M18" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Forest</v>
+      </c>
+      <c r="N18" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Happy</v>
+      </c>
+      <c r="O18" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P18" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" ht="17">
       <c r="B19" s="2" t="s">
         <v>67</v>
       </c>
@@ -1026,31 +1317,123 @@
       <c r="I19" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" ht="17">
+      <c r="M19" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Forest</v>
+      </c>
+      <c r="N19" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Happy</v>
+      </c>
+      <c r="O19" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P19" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" ht="17">
       <c r="B20" s="2" t="s">
         <v>61</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" ht="34">
+      <c r="I20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M20" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Black</v>
+      </c>
+      <c r="N20" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Happy</v>
+      </c>
+      <c r="O20" s="1">
+        <f t="shared" si="2"/>
+        <v>-500</v>
+      </c>
+      <c r="P20" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="34">
       <c r="B21" s="2" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" ht="17">
+      <c r="I21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M21" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Black</v>
+      </c>
+      <c r="N21" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Happy</v>
+      </c>
+      <c r="O21" s="1">
+        <f t="shared" si="2"/>
+        <v>-500</v>
+      </c>
+      <c r="P21" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" ht="17">
       <c r="B22" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" ht="34">
+      <c r="I22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M22" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Black</v>
+      </c>
+      <c r="N22" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Happy</v>
+      </c>
+      <c r="O22" s="1">
+        <f t="shared" si="2"/>
+        <v>-500</v>
+      </c>
+      <c r="P22" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" ht="34">
       <c r="B23" s="2" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" ht="34">
+      <c r="I23" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M23" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Black</v>
+      </c>
+      <c r="N23" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Happy</v>
+      </c>
+      <c r="O23" s="1">
+        <f t="shared" si="2"/>
+        <v>-500</v>
+      </c>
+      <c r="P23" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" ht="34">
       <c r="B24" s="2" t="s">
         <v>45</v>
       </c>
@@ -1060,8 +1443,27 @@
       <c r="G24" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" ht="34">
+      <c r="I24" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M24" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Black</v>
+      </c>
+      <c r="N24" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Happy</v>
+      </c>
+      <c r="O24" s="1">
+        <f t="shared" si="2"/>
+        <v>-500</v>
+      </c>
+      <c r="P24" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" ht="34">
       <c r="B25" s="2" t="s">
         <v>70</v>
       </c>
@@ -1077,13 +1479,48 @@
       <c r="I25" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" ht="17">
+      <c r="M25" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Black</v>
+      </c>
+      <c r="N25" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Happy</v>
+      </c>
+      <c r="O25" s="1">
+        <f t="shared" si="2"/>
+        <v>-500</v>
+      </c>
+      <c r="P25" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" ht="17">
       <c r="B26" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" ht="17">
+      <c r="I26" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M26" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Black</v>
+      </c>
+      <c r="N26" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Happy</v>
+      </c>
+      <c r="O26" s="1">
+        <f t="shared" si="2"/>
+        <v>-500</v>
+      </c>
+      <c r="P26" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" ht="17">
       <c r="A27" s="2" t="s">
         <v>0</v>
       </c>
@@ -1102,8 +1539,27 @@
       <c r="G27" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" ht="17">
+      <c r="I27" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M27" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Black</v>
+      </c>
+      <c r="N27" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Happy</v>
+      </c>
+      <c r="O27" s="1">
+        <f t="shared" si="2"/>
+        <v>-500</v>
+      </c>
+      <c r="P27" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" ht="17">
       <c r="A28" s="2" t="s">
         <v>1</v>
       </c>
@@ -1116,8 +1572,24 @@
       <c r="D28" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" ht="17">
+      <c r="M28" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Forest</v>
+      </c>
+      <c r="N28" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Happy</v>
+      </c>
+      <c r="O28" s="1">
+        <f t="shared" si="2"/>
+        <v>-500</v>
+      </c>
+      <c r="P28" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" ht="17">
       <c r="A29" s="2" t="s">
         <v>0</v>
       </c>
@@ -1139,8 +1611,24 @@
       <c r="I29" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" ht="17">
+      <c r="M29" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Forest</v>
+      </c>
+      <c r="N29" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Happy</v>
+      </c>
+      <c r="O29" s="1">
+        <f t="shared" si="2"/>
+        <v>-500</v>
+      </c>
+      <c r="P29" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" ht="17">
       <c r="A30" s="2" t="s">
         <v>0</v>
       </c>
@@ -1153,8 +1641,27 @@
       <c r="D30" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" ht="17">
+      <c r="I30" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="M30" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Forest</v>
+      </c>
+      <c r="N30" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Happy</v>
+      </c>
+      <c r="O30" s="1">
+        <f t="shared" si="2"/>
+        <v>-1000</v>
+      </c>
+      <c r="P30" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" ht="17">
       <c r="A31" s="2" t="s">
         <v>1</v>
       </c>
@@ -1170,8 +1677,27 @@
       <c r="G31" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" ht="34">
+      <c r="I31" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="M31" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Forest</v>
+      </c>
+      <c r="N31" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Happy</v>
+      </c>
+      <c r="O31" s="1">
+        <f t="shared" si="2"/>
+        <v>-1000</v>
+      </c>
+      <c r="P31" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" ht="34">
       <c r="A32" s="2" t="s">
         <v>1</v>
       </c>
@@ -1184,8 +1710,24 @@
       <c r="D32" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" ht="17">
+      <c r="M32" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Forest</v>
+      </c>
+      <c r="N32" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Happy</v>
+      </c>
+      <c r="O32" s="1">
+        <f t="shared" si="2"/>
+        <v>-1000</v>
+      </c>
+      <c r="P32" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" ht="17">
       <c r="B33" s="2" t="s">
         <v>53</v>
       </c>
@@ -1195,29 +1737,93 @@
       <c r="E33" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" ht="17">
+      <c r="M33" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Forest</v>
+      </c>
+      <c r="N33" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Happy</v>
+      </c>
+      <c r="O33" s="1">
+        <f t="shared" si="2"/>
+        <v>-1000</v>
+      </c>
+      <c r="P33" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" ht="17">
       <c r="B34" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" ht="17">
+      <c r="M34" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Sky</v>
+      </c>
+      <c r="N34" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Happy</v>
+      </c>
+      <c r="O34" s="1">
+        <f t="shared" si="2"/>
+        <v>-1000</v>
+      </c>
+      <c r="P34" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" ht="17">
       <c r="B35" s="2" t="s">
         <v>55</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" ht="17">
+      <c r="M35" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Sky</v>
+      </c>
+      <c r="N35" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Happy</v>
+      </c>
+      <c r="O35" s="1">
+        <f t="shared" si="2"/>
+        <v>-1000</v>
+      </c>
+      <c r="P35" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" ht="17">
       <c r="B36" s="2" t="s">
         <v>56</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" ht="17">
+      <c r="M36" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Sky</v>
+      </c>
+      <c r="N36" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Happy</v>
+      </c>
+      <c r="O36" s="1">
+        <f t="shared" si="2"/>
+        <v>-1000</v>
+      </c>
+      <c r="P36" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" ht="17">
       <c r="A37" s="2" t="s">
         <v>1</v>
       </c>
@@ -1242,8 +1848,24 @@
       <c r="I37" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" ht="17">
+      <c r="M37" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Sky</v>
+      </c>
+      <c r="N37" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Happy</v>
+      </c>
+      <c r="O37" s="1">
+        <f t="shared" si="2"/>
+        <v>-1000</v>
+      </c>
+      <c r="P37" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" ht="17">
       <c r="A38" s="2" t="s">
         <v>0</v>
       </c>
@@ -1256,8 +1878,27 @@
       <c r="D38" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" ht="17">
+      <c r="I38" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M38" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Forest</v>
+      </c>
+      <c r="N38" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Happy</v>
+      </c>
+      <c r="O38" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P38" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" ht="17">
       <c r="A39" s="2" t="s">
         <v>1</v>
       </c>
@@ -1273,16 +1914,51 @@
       <c r="G39" s="1" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" ht="17">
+      <c r="I39" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M39" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Forest</v>
+      </c>
+      <c r="N39" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Happy</v>
+      </c>
+      <c r="O39" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P39" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" ht="17">
       <c r="B40" s="2" t="s">
         <v>57</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" ht="34">
+      <c r="M40" s="1" t="str">
+        <f>IF(E39&lt;&gt;"",E39,M39)</f>
+        <v>Forest</v>
+      </c>
+      <c r="N40" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Happy</v>
+      </c>
+      <c r="O40" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P40" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" ht="34">
       <c r="B41" s="2" t="s">
         <v>72</v>
       </c>
@@ -1295,16 +1971,48 @@
       <c r="F41" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" ht="34">
+      <c r="M41" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Forest</v>
+      </c>
+      <c r="N41" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Happy</v>
+      </c>
+      <c r="O41" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P41" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" ht="34">
       <c r="B42" s="2" t="s">
         <v>74</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" ht="17">
+      <c r="M42" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Bridge-Connect</v>
+      </c>
+      <c r="N42" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Waterfall</v>
+      </c>
+      <c r="O42" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P42" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" ht="17">
       <c r="A43" s="2" t="s">
         <v>1</v>
       </c>
@@ -1326,16 +2034,51 @@
       <c r="I43" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" ht="34">
+      <c r="M43" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Bridge-Connect</v>
+      </c>
+      <c r="N43" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Waterfall</v>
+      </c>
+      <c r="O43" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P43" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" ht="34">
       <c r="B44" s="2" t="s">
         <v>76</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" ht="17">
+      <c r="I44" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M44" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Bridge-Connect</v>
+      </c>
+      <c r="N44" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Waterfall</v>
+      </c>
+      <c r="O44" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P44" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" ht="17">
       <c r="A45" s="2" t="s">
         <v>0</v>
       </c>
@@ -1351,8 +2094,27 @@
       <c r="G45" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" ht="17">
+      <c r="I45" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M45" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Bridge-Connect</v>
+      </c>
+      <c r="N45" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Waterfall</v>
+      </c>
+      <c r="O45" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P45" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" ht="17">
       <c r="A46" s="2" t="s">
         <v>1</v>
       </c>
@@ -1365,8 +2127,24 @@
       <c r="D46" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" ht="17">
+      <c r="M46" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Bridge-Connect</v>
+      </c>
+      <c r="N46" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Waterfall</v>
+      </c>
+      <c r="O46" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P46" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" ht="17">
       <c r="A47" s="2" t="s">
         <v>21</v>
       </c>

</xml_diff>

<commit_message>
4.27 Finish History System
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/StoryScript.xlsx
+++ b/Assets/StreamingAssets/StoryScript.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/renqi/TextAdvancedGame/Assets/StreamingAssets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A468C65E-CA6B-0E48-B367-D8685845FEE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A634C762-58C8-2743-9332-1D0A883C54C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15760" xr2:uid="{4FF494A4-B03B-D144-A30E-F081D1418406}"/>
   </bookViews>
@@ -169,10 +169,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>The first is "Reflected Falls."</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>A waterfall plunges straight down near the manor, its spray shimmering as it meets the water below, like light and shadow flickering into view.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -382,6 +378,10 @@
   </si>
   <si>
     <t>LastX2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The first is &lt;i&gt;&lt;color=#D93025&gt;Reflected Falls&lt;/color&gt;&lt;/i&gt;.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -774,8 +774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40E189AB-F231-6C46-8064-720ADE40C742}">
   <dimension ref="A1:P47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B26" workbookViewId="0">
-      <selection activeCell="J49" sqref="J49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -834,21 +834,21 @@
         <v>14</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="17">
       <c r="B2" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>22</v>
@@ -857,7 +857,7 @@
         <v>12</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="34">
@@ -934,7 +934,7 @@
     </row>
     <row r="6" spans="1:16" ht="17">
       <c r="B6" s="2" t="s">
-        <v>33</v>
+        <v>86</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>22</v>
@@ -958,7 +958,7 @@
     </row>
     <row r="7" spans="1:16" ht="34">
       <c r="B7" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M7" s="1" t="str">
         <f t="shared" si="0"/>
@@ -979,7 +979,7 @@
     </row>
     <row r="8" spans="1:16" ht="17">
       <c r="B8" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>22</v>
@@ -1003,7 +1003,7 @@
     </row>
     <row r="9" spans="1:16" ht="34">
       <c r="B9" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M9" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1024,7 +1024,7 @@
     </row>
     <row r="10" spans="1:16" ht="34">
       <c r="B10" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>22</v>
@@ -1051,7 +1051,7 @@
         <v>0</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>4</v>
@@ -1078,7 +1078,7 @@
     </row>
     <row r="12" spans="1:16" ht="34">
       <c r="B12" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>22</v>
@@ -1105,7 +1105,7 @@
         <v>0</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>4</v>
@@ -1132,7 +1132,7 @@
     </row>
     <row r="14" spans="1:16" ht="17">
       <c r="B14" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>4</v>
@@ -1162,7 +1162,7 @@
         <v>1</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>2</v>
@@ -1201,7 +1201,7 @@
         <v>0</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>3</v>
@@ -1234,7 +1234,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>23</v>
@@ -1270,7 +1270,7 @@
     </row>
     <row r="18" spans="1:16" ht="34">
       <c r="B18" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>22</v>
@@ -1300,7 +1300,7 @@
     </row>
     <row r="19" spans="1:16" ht="17">
       <c r="B19" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>22</v>
@@ -1336,7 +1336,7 @@
     </row>
     <row r="20" spans="1:16" ht="17">
       <c r="B20" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>22</v>
@@ -1363,7 +1363,7 @@
     </row>
     <row r="21" spans="1:16" ht="34">
       <c r="B21" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>23</v>
@@ -1387,7 +1387,7 @@
     </row>
     <row r="22" spans="1:16" ht="17">
       <c r="B22" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>23</v>
@@ -1411,7 +1411,7 @@
     </row>
     <row r="23" spans="1:16" ht="34">
       <c r="B23" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>23</v>
@@ -1435,7 +1435,7 @@
     </row>
     <row r="24" spans="1:16" ht="34">
       <c r="B24" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>22</v>
@@ -1465,7 +1465,7 @@
     </row>
     <row r="25" spans="1:16" ht="34">
       <c r="B25" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>22</v>
@@ -1498,7 +1498,7 @@
     </row>
     <row r="26" spans="1:16" ht="17">
       <c r="B26" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>4</v>
@@ -1525,7 +1525,7 @@
         <v>0</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>24</v>
@@ -1564,7 +1564,7 @@
         <v>1</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>23</v>
@@ -1594,7 +1594,7 @@
         <v>0</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>24</v>
@@ -1609,7 +1609,7 @@
         <v>-1000</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="M29" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1633,7 +1633,7 @@
         <v>0</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>25</v>
@@ -1642,7 +1642,7 @@
         <v>22</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="M30" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1666,7 +1666,7 @@
         <v>1</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>2</v>
@@ -1678,7 +1678,7 @@
         <v>15</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="M31" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1702,7 +1702,7 @@
         <v>1</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>2</v>
@@ -1729,7 +1729,7 @@
     </row>
     <row r="33" spans="1:16" ht="17">
       <c r="B33" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>22</v>
@@ -1756,7 +1756,7 @@
     </row>
     <row r="34" spans="1:16" ht="17">
       <c r="B34" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M34" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1777,7 +1777,7 @@
     </row>
     <row r="35" spans="1:16" ht="17">
       <c r="B35" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>22</v>
@@ -1801,7 +1801,7 @@
     </row>
     <row r="36" spans="1:16" ht="17">
       <c r="B36" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>22</v>
@@ -1828,7 +1828,7 @@
         <v>1</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>23</v>
@@ -1870,7 +1870,7 @@
         <v>0</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>28</v>
@@ -1903,7 +1903,7 @@
         <v>1</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>23</v>
@@ -1912,7 +1912,7 @@
         <v>5</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I39" s="1" t="s">
         <v>23</v>
@@ -1936,7 +1936,7 @@
     </row>
     <row r="40" spans="1:16" ht="17">
       <c r="B40" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>22</v>
@@ -1960,7 +1960,7 @@
     </row>
     <row r="41" spans="1:16" ht="34">
       <c r="B41" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>22</v>
@@ -1969,7 +1969,7 @@
         <v>29</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M41" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1990,7 +1990,7 @@
     </row>
     <row r="42" spans="1:16" ht="34">
       <c r="B42" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>22</v>
@@ -2017,7 +2017,7 @@
         <v>1</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>2</v>
@@ -2053,7 +2053,7 @@
     </row>
     <row r="44" spans="1:16" ht="34">
       <c r="B44" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>22</v>
@@ -2083,7 +2083,7 @@
         <v>0</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>24</v>
@@ -2119,7 +2119,7 @@
         <v>1</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>2</v>
@@ -2149,16 +2149,16 @@
         <v>21</v>
       </c>
       <c r="B47" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C47" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C47" s="1" t="s">
-        <v>82</v>
-      </c>
       <c r="D47" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
5.17 Finish Gallery System
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/StoryScript.xlsx
+++ b/Assets/StreamingAssets/StoryScript.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/renqi/TextAdvancedGame/Assets/StreamingAssets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE16E229-6AF3-4541-8DCD-2C9098E72997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BA34A82-98FA-B842-A9D5-07D9B47D8D6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15760" xr2:uid="{4FF494A4-B03B-D144-A30E-F081D1418406}"/>
   </bookViews>
@@ -385,11 +385,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>BlackMask</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>HistoryAction</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>History1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -783,7 +783,7 @@
   <dimension ref="A1:R47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="S18" sqref="S18"/>
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -859,7 +859,7 @@
         <v>86</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="17">
@@ -1062,7 +1062,7 @@
         <v>0</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="R10" s="1" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
5.20 Advance the Story
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/StoryScript.xlsx
+++ b/Assets/StreamingAssets/StoryScript.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/renqi/TextAdvancedGame/Assets/StreamingAssets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BA34A82-98FA-B842-A9D5-07D9B47D8D6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E00DAB49-D18E-8F48-AEF3-7CCD061717E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15760" xr2:uid="{4FF494A4-B03B-D144-A30E-F081D1418406}"/>
   </bookViews>
@@ -782,7 +782,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40E189AB-F231-6C46-8064-720ADE40C742}">
   <dimension ref="A1:R47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
5.29 Optimise History System
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/StoryScript.xlsx
+++ b/Assets/StreamingAssets/StoryScript.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/renqi/TextAdvancedGame/Assets/StreamingAssets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E00DAB49-D18E-8F48-AEF3-7CCD061717E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3659303-0708-224F-867B-298B33F90135}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15760" xr2:uid="{4FF494A4-B03B-D144-A30E-F081D1418406}"/>
+    <workbookView xWindow="0" yWindow="1300" windowWidth="28800" windowHeight="16080" xr2:uid="{4FF494A4-B03B-D144-A30E-F081D1418406}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="89">
   <si>
     <t>Yao</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -157,50 +157,14 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>It is a grand compound nestled in the upper reaches of the Gong River, embraced by towering slopes and cliffs. Locals simply call it Qingliu Manor.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Though sparsely populated, the upper Gong River is famed far and wide for its breathtaking mountain views.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Among its most celebrated sights are three scenic wonders—</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>A waterfall plunges straight down near the manor, its spray shimmering as it meets the water below, like light and shadow flickering into view.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>The second is "Spring Songs in the Forked Valley."</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Where the mountain path splits, birdsong echoes through the ravine. It's a treasured spot for listening to the chorus of spring.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>So really, how could we pass through Gongjiang County and not pay a visit to the famed Qingliu Manor?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Sir, wait a moment…</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>I had been quietly listening this whole time, but now that the story seemed to be ending, I couldn’t help but interject.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Weren’t there supposed to be three famous sights? You only mentioned two…</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>What’s the last one?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Three named, two listed—that’s just one of those unwritten rules, isn’t it?</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -213,14 +177,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>On the way to his new post, Master proposed a detour to the Gong River to take in the famed lakes and mountains along the way.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Yao Chong, at your service.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Sir, how much farther is Qingliu Manor? It feels like we’ve been walking forever…</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -245,26 +201,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>He always sounds so confident. I sigh and lift my head—</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Through the thick foliage above, I glimpse a sliver of gray sky.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>My skin and nose tell me the mountain air is so humid it might wring water if squeezed.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Looks like a storm is coming.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>I push aside the branches ahead of us, half in doubt. And see…</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>We’ve arrived.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -277,14 +213,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Before traveling to court, he served at the Court of Judicature and Revision</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Where he handled criminal cases with absolute fairness—over seventeen thousand verdicts in a single year, and not a single wrongful conviction.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Happy</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -293,51 +221,14 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>That’s how Sir is. After all these years traveling with him, I’m fairly certain he just forgot what the third one was.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>My Sir’s name is Judge Dee.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>A few weeks ago, he offended Wu Sansi, the emperor’s favored consort's nephew, and was demoted to serve as magistrate of Pengyang County.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">But alas, Sir is upright and uncompromising. </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>And I—
-I'm his student and bodyguard.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>The Riverworks Estate of Gongjiang County.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>A worn wooden suspension bridge, swaying gently, stretching across a vast chasm—linking two cliffs some dozens of meters apart.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Q1C2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Just beyond the suspension bridge, a mighty waterfall thundered down the cliffside, its roaring waters deafening to the ear.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>I told you not to worry. Once we cross this bridge, we’ll be at Qingliu Manor.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>I followed Master’s finger, and only then did I spot the faint outline of the manor walls, barely visible in the distant mist.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Why would they build the Riverworks Estate so high up the mountain?</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -377,10 +268,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>The first is &lt;i&gt;&lt;color=#D93025&gt;Reflected Falls&lt;/color&gt;&lt;/i&gt;.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>History</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -390,6 +277,119 @@
   </si>
   <si>
     <t>History1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;color=#00CC00&gt;(The Riverworks Estate of Gongjiang County.)&lt;/color&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;color=#00CC00&gt;(It is a grand compound nestled in the upper reaches of the Gong River, embraced by towering slopes and cliffs. Locals simply call it Qingliu Manor.)&lt;/color&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;color=#00CC00&gt;(Though sparsely populated, the upper Gong River is famed far and wide for its breathtaking mountain views.)&lt;/color&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;color=#00CC00&gt;(Among its most celebrated sights are three scenic wonders—)&lt;/color&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;color=#00CC00&gt;(The first is &lt;i&gt;&lt;color=#D93025&gt;Reflected Falls&lt;/color&gt;&lt;/i&gt;.)&lt;/color&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;color=#00CC00&gt;(A waterfall plunges straight down near the manor, its spray shimmering as it meets the water below, like light and shadow flickering into view.)&lt;/color&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;color=#00CC00&gt;(The second is "Spring Songs in the Forked Valley.")&lt;/color&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;color=#00CC00&gt;(Where the mountain path splits, birdsong echoes through the ravine. It's a treasured spot for listening to the chorus of spring.)&lt;/color&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;color=#00CC00&gt;(So really, how could we pass through Gongjiang County and not pay a visit to the famed Qingliu Manor?)&lt;/color&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;color=#00CC00&gt;(I had been quietly listening this whole time, but now that the story seemed to be ending, I couldn’t help but interject.)&lt;/color&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;color=#00CC00&gt;(What’s the last one?)&lt;/color&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;color=#00CC00&gt;(That’s how Sir is. After all these years traveling with him, I’m fairly certain he just forgot what the third one was.)&lt;/color&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;color=#00CC00&gt;(My Sir’s name is Judge Dee.)&lt;/color&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;color=#00CC00&gt;(Before traveling to court, he served at the Court of Judicature and Revision)&lt;/color&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;color=#00CC00&gt;(Where he handled criminal cases with absolute fairness—over seventeen thousand verdicts in a single year, and not a single wrongful conviction.)&lt;/color&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;color=#00CC00&gt;(But alas, Sir is upright and uncompromising. )&lt;/color&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;color=#00CC00&gt;(A few weeks ago, he offended Wu Sansi, the emperor’s favored consort's nephew, and was demoted to serve as magistrate of Pengyang County.)&lt;/color&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;color=#00CC00&gt;(On the way to his new post, Master proposed a detour to the Gong River to take in the famed lakes and mountains along the way.)&lt;/color&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;color=#00CC00&gt;(And I—
+I'm his student and bodyguard.)&lt;/color&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;color=#00CC00&gt;(Yao Chong, at your service.)&lt;/color&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;color=#00CC00&gt;(He always sounds so confident. I sigh and lift my head—)&lt;/color&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;color=#00CC00&gt;(Through the thick foliage above, I glimpse a sliver of gray sky.)&lt;/color&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;color=#00CC00&gt;(My skin and nose tell me the mountain air is so humid it might wring water if squeezed.)&lt;/color&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;color=#00CC00&gt;(Looks like a storm is coming.)&lt;/color&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;color=#00CC00&gt;(I push aside the branches ahead of us, half in doubt. And see…)&lt;/color&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;color=#00CC00&gt;(A worn wooden suspension bridge, swaying gently, stretching across a vast chasm—linking two cliffs some dozens of meters apart.)&lt;/color&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;color=#00CC00&gt;(Just beyond the suspension bridge, a mighty waterfall thundered down the cliffside, its roaring waters deafening to the ear.)&lt;/color&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;color=#00CC00&gt;(I followed Master’s finger, and only then did I spot the faint outline of the manor walls, barely visible in the distant mist.)&lt;/color&gt;</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -414,12 +414,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -436,7 +448,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -445,6 +457,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -782,8 +800,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40E189AB-F231-6C46-8064-720ADE40C742}">
   <dimension ref="A1:R47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -799,7 +817,7 @@
     <col min="9" max="9" width="18.83203125" style="1" customWidth="1"/>
     <col min="10" max="10" width="14.33203125" style="1" customWidth="1"/>
     <col min="11" max="11" width="9" style="1" customWidth="1"/>
-    <col min="12" max="12" width="13.5" style="1" customWidth="1"/>
+    <col min="12" max="12" width="19.33203125" style="1" customWidth="1"/>
     <col min="13" max="13" width="18.33203125" style="1" customWidth="1"/>
     <col min="14" max="17" width="10.83203125" style="1"/>
     <col min="18" max="18" width="16.33203125" style="1" customWidth="1"/>
@@ -844,27 +862,27 @@
         <v>14</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>81</v>
+        <v>54</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>82</v>
+        <v>55</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>83</v>
+        <v>56</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>84</v>
+        <v>57</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>86</v>
+        <v>58</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>87</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="17">
       <c r="B2" s="2" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>22</v>
@@ -873,12 +891,12 @@
         <v>12</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="34">
       <c r="B3" s="2" t="s">
-        <v>30</v>
+        <v>62</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>22</v>
@@ -902,7 +920,7 @@
     </row>
     <row r="4" spans="1:18" ht="34">
       <c r="B4" s="2" t="s">
-        <v>31</v>
+        <v>63</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>22</v>
@@ -926,7 +944,7 @@
     </row>
     <row r="5" spans="1:18" ht="17">
       <c r="B5" s="2" t="s">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>22</v>
@@ -950,7 +968,7 @@
     </row>
     <row r="6" spans="1:18" ht="17">
       <c r="B6" s="2" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>22</v>
@@ -974,7 +992,10 @@
     </row>
     <row r="7" spans="1:18" ht="34">
       <c r="B7" s="2" t="s">
-        <v>33</v>
+        <v>66</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="M7" s="1" t="str">
         <f t="shared" si="0"/>
@@ -995,7 +1016,7 @@
     </row>
     <row r="8" spans="1:18" ht="17">
       <c r="B8" s="2" t="s">
-        <v>34</v>
+        <v>67</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>22</v>
@@ -1019,7 +1040,10 @@
     </row>
     <row r="9" spans="1:18" ht="34">
       <c r="B9" s="2" t="s">
-        <v>35</v>
+        <v>68</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="M9" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1040,10 +1064,10 @@
     </row>
     <row r="10" spans="1:18" ht="34">
       <c r="B10" s="2" t="s">
-        <v>36</v>
+        <v>69</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="M10" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1062,7 +1086,7 @@
         <v>0</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>88</v>
+        <v>60</v>
       </c>
       <c r="R10" s="1" t="s">
         <v>18</v>
@@ -1073,7 +1097,7 @@
         <v>0</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>4</v>
@@ -1081,6 +1105,15 @@
       <c r="D11" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="J11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K11" s="3">
+        <v>500</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="M11" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Forest</v>
@@ -1100,11 +1133,14 @@
     </row>
     <row r="12" spans="1:18" ht="34">
       <c r="B12" s="2" t="s">
-        <v>38</v>
+        <v>70</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
       <c r="M12" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Forest</v>
@@ -1119,7 +1155,7 @@
       </c>
       <c r="P12" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>500</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="17">
@@ -1127,7 +1163,7 @@
         <v>0</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>4</v>
@@ -1135,6 +1171,9 @@
       <c r="D13" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
       <c r="M13" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Forest</v>
@@ -1149,12 +1188,12 @@
       </c>
       <c r="P13" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>500</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="17">
       <c r="B14" s="2" t="s">
-        <v>40</v>
+        <v>71</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>4</v>
@@ -1162,6 +1201,11 @@
       <c r="D14" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="J14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
       <c r="M14" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Forest</v>
@@ -1176,7 +1220,7 @@
       </c>
       <c r="P14" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="R14" s="1" t="s">
         <v>15</v>
@@ -1187,7 +1231,7 @@
         <v>1</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>2</v>
@@ -1195,13 +1239,13 @@
       <c r="D15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="G15" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H15" s="1">
-        <v>0</v>
-      </c>
-      <c r="I15" s="1" t="s">
+      <c r="H15" s="4">
+        <v>-500</v>
+      </c>
+      <c r="I15" s="4" t="s">
         <v>2</v>
       </c>
       <c r="M15" s="1" t="str">
@@ -1218,7 +1262,7 @@
       </c>
       <c r="P15" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>500</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="17">
@@ -1226,7 +1270,7 @@
         <v>0</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>3</v>
@@ -1234,9 +1278,9 @@
       <c r="D16" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I16" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
       <c r="M16" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Forest</v>
@@ -1247,11 +1291,11 @@
       </c>
       <c r="O16" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-500</v>
       </c>
       <c r="P16" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>500</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="17">
@@ -1259,7 +1303,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>23</v>
@@ -1267,15 +1311,9 @@
       <c r="D17" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G17" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H17" s="1">
-        <v>0</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>23</v>
-      </c>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
       <c r="M17" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Forest</v>
@@ -1286,26 +1324,25 @@
       </c>
       <c r="O17" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-500</v>
       </c>
       <c r="P17" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>500</v>
       </c>
     </row>
     <row r="18" spans="1:16" ht="34">
       <c r="B18" s="2" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="G18" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="I18" s="1" t="s">
-        <v>23</v>
-      </c>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
       <c r="M18" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Forest</v>
@@ -1316,16 +1353,16 @@
       </c>
       <c r="O18" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-500</v>
       </c>
       <c r="P18" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>500</v>
       </c>
     </row>
     <row r="19" spans="1:16" ht="17">
       <c r="B19" s="2" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>22</v>
@@ -1333,13 +1370,13 @@
       <c r="E19" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="G19" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H19" s="1">
+      <c r="H19" s="4">
         <v>-500</v>
       </c>
-      <c r="I19" s="1" t="s">
+      <c r="I19" s="4" t="s">
         <v>23</v>
       </c>
       <c r="M19" s="1" t="str">
@@ -1352,23 +1389,23 @@
       </c>
       <c r="O19" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-500</v>
       </c>
       <c r="P19" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" ht="17">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" ht="34">
       <c r="B20" s="2" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I20" s="1" t="s">
-        <v>23</v>
-      </c>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
       <c r="M20" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Black</v>
@@ -1383,16 +1420,19 @@
       </c>
       <c r="P20" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>500</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="34">
       <c r="B21" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>23</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
       <c r="M21" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Black</v>
@@ -1407,16 +1447,19 @@
       </c>
       <c r="P21" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>500</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="17">
       <c r="B22" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>23</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
       <c r="M22" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Black</v>
@@ -1431,16 +1474,19 @@
       </c>
       <c r="P22" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>500</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="34">
       <c r="B23" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>23</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
       <c r="M23" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Black</v>
@@ -1455,22 +1501,21 @@
       </c>
       <c r="P23" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>500</v>
       </c>
     </row>
     <row r="24" spans="1:16" ht="34">
       <c r="B24" s="2" t="s">
-        <v>44</v>
+        <v>78</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G24" s="1" t="s">
+      <c r="G24" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="I24" s="1" t="s">
-        <v>23</v>
-      </c>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
       <c r="M24" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Black</v>
@@ -1485,49 +1530,64 @@
       </c>
       <c r="P24" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>500</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="34">
       <c r="B25" s="2" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G25" s="1" t="s">
+      <c r="G25" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H25" s="1">
+      <c r="H25" s="4">
+        <v>0</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K25" s="3">
+        <v>0</v>
+      </c>
+      <c r="L25" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M25" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Black</v>
+      </c>
+      <c r="N25" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Happy</v>
+      </c>
+      <c r="O25" s="1">
+        <f t="shared" si="2"/>
         <v>-500</v>
       </c>
-      <c r="I25" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="M25" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Black</v>
-      </c>
-      <c r="N25" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Happy</v>
-      </c>
-      <c r="O25" s="1">
-        <f t="shared" si="2"/>
-        <v>-500</v>
-      </c>
       <c r="P25" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>500</v>
       </c>
     </row>
     <row r="26" spans="1:16" ht="17">
       <c r="B26" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>4</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
       <c r="M26" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Black</v>
@@ -1538,7 +1598,7 @@
       </c>
       <c r="O26" s="1">
         <f t="shared" si="2"/>
-        <v>-500</v>
+        <v>0</v>
       </c>
       <c r="P26" s="1">
         <f t="shared" si="3"/>
@@ -1550,7 +1610,7 @@
         <v>0</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>24</v>
@@ -1561,12 +1621,12 @@
       <c r="E27" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G27" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
       <c r="M27" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Black</v>
@@ -1577,7 +1637,7 @@
       </c>
       <c r="O27" s="1">
         <f t="shared" si="2"/>
-        <v>-500</v>
+        <v>0</v>
       </c>
       <c r="P27" s="1">
         <f t="shared" si="3"/>
@@ -1589,7 +1649,7 @@
         <v>1</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>23</v>
@@ -1597,6 +1657,12 @@
       <c r="D28" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
       <c r="M28" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Forest</v>
@@ -1607,7 +1673,7 @@
       </c>
       <c r="O28" s="1">
         <f t="shared" si="2"/>
-        <v>-500</v>
+        <v>0</v>
       </c>
       <c r="P28" s="1">
         <f t="shared" si="3"/>
@@ -1619,7 +1685,7 @@
         <v>0</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>24</v>
@@ -1627,15 +1693,12 @@
       <c r="D29" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G29" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H29" s="1">
-        <v>-1000</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>63</v>
-      </c>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
       <c r="M29" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Forest</v>
@@ -1646,7 +1709,7 @@
       </c>
       <c r="O29" s="1">
         <f t="shared" si="2"/>
-        <v>-500</v>
+        <v>0</v>
       </c>
       <c r="P29" s="1">
         <f t="shared" si="3"/>
@@ -1658,7 +1721,7 @@
         <v>0</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>25</v>
@@ -1666,9 +1729,12 @@
       <c r="D30" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I30" s="1" t="s">
-        <v>63</v>
-      </c>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
       <c r="M30" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Forest</v>
@@ -1679,7 +1745,7 @@
       </c>
       <c r="O30" s="1">
         <f t="shared" si="2"/>
-        <v>-1000</v>
+        <v>0</v>
       </c>
       <c r="P30" s="1">
         <f t="shared" si="3"/>
@@ -1691,7 +1757,7 @@
         <v>1</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>2</v>
@@ -1699,12 +1765,12 @@
       <c r="D31" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G31" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I31" s="1" t="s">
-        <v>63</v>
-      </c>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
       <c r="M31" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Forest</v>
@@ -1715,7 +1781,7 @@
       </c>
       <c r="O31" s="1">
         <f t="shared" si="2"/>
-        <v>-1000</v>
+        <v>0</v>
       </c>
       <c r="P31" s="1">
         <f t="shared" si="3"/>
@@ -1727,7 +1793,7 @@
         <v>1</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>2</v>
@@ -1735,6 +1801,12 @@
       <c r="D32" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
       <c r="M32" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Forest</v>
@@ -1745,7 +1817,7 @@
       </c>
       <c r="O32" s="1">
         <f t="shared" si="2"/>
-        <v>-1000</v>
+        <v>0</v>
       </c>
       <c r="P32" s="1">
         <f t="shared" si="3"/>
@@ -1754,7 +1826,7 @@
     </row>
     <row r="33" spans="1:16" ht="17">
       <c r="B33" s="2" t="s">
-        <v>52</v>
+        <v>81</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>22</v>
@@ -1762,6 +1834,16 @@
       <c r="E33" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="G33" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H33" s="4"/>
+      <c r="I33" s="4"/>
+      <c r="J33" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K33" s="3"/>
+      <c r="L33" s="3"/>
       <c r="M33" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Forest</v>
@@ -1772,7 +1854,7 @@
       </c>
       <c r="O33" s="1">
         <f t="shared" si="2"/>
-        <v>-1000</v>
+        <v>0</v>
       </c>
       <c r="P33" s="1">
         <f t="shared" si="3"/>
@@ -1781,7 +1863,10 @@
     </row>
     <row r="34" spans="1:16" ht="17">
       <c r="B34" s="2" t="s">
-        <v>53</v>
+        <v>82</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="M34" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1793,16 +1878,16 @@
       </c>
       <c r="O34" s="1">
         <f t="shared" si="2"/>
-        <v>-1000</v>
+        <v>0</v>
       </c>
       <c r="P34" s="1">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:16" ht="17">
+    <row r="35" spans="1:16" ht="34">
       <c r="B35" s="2" t="s">
-        <v>54</v>
+        <v>83</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>22</v>
@@ -1817,7 +1902,7 @@
       </c>
       <c r="O35" s="1">
         <f t="shared" si="2"/>
-        <v>-1000</v>
+        <v>0</v>
       </c>
       <c r="P35" s="1">
         <f t="shared" si="3"/>
@@ -1826,7 +1911,7 @@
     </row>
     <row r="36" spans="1:16" ht="17">
       <c r="B36" s="2" t="s">
-        <v>55</v>
+        <v>84</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>22</v>
@@ -1841,7 +1926,7 @@
       </c>
       <c r="O36" s="1">
         <f t="shared" si="2"/>
-        <v>-1000</v>
+        <v>0</v>
       </c>
       <c r="P36" s="1">
         <f t="shared" si="3"/>
@@ -1853,7 +1938,7 @@
         <v>1</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>23</v>
@@ -1864,13 +1949,13 @@
       <c r="E37" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G37" s="1" t="s">
+      <c r="G37" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H37" s="1">
-        <v>0</v>
-      </c>
-      <c r="I37" s="1" t="s">
+      <c r="H37" s="4">
+        <v>-500</v>
+      </c>
+      <c r="I37" s="4" t="s">
         <v>23</v>
       </c>
       <c r="M37" s="1" t="str">
@@ -1883,7 +1968,7 @@
       </c>
       <c r="O37" s="1">
         <f t="shared" si="2"/>
-        <v>-1000</v>
+        <v>0</v>
       </c>
       <c r="P37" s="1">
         <f t="shared" si="3"/>
@@ -1895,7 +1980,7 @@
         <v>0</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>28</v>
@@ -1903,9 +1988,9 @@
       <c r="D38" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I38" s="1" t="s">
-        <v>23</v>
-      </c>
+      <c r="G38" s="4"/>
+      <c r="H38" s="4"/>
+      <c r="I38" s="4"/>
       <c r="M38" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Forest</v>
@@ -1916,7 +2001,7 @@
       </c>
       <c r="O38" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-500</v>
       </c>
       <c r="P38" s="1">
         <f t="shared" si="3"/>
@@ -1928,7 +2013,7 @@
         <v>1</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>23</v>
@@ -1936,10 +2021,11 @@
       <c r="D39" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G39" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="I39" s="1" t="s">
+      <c r="G39" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H39" s="4"/>
+      <c r="I39" s="4" t="s">
         <v>23</v>
       </c>
       <c r="M39" s="1" t="str">
@@ -1952,7 +2038,7 @@
       </c>
       <c r="O39" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-500</v>
       </c>
       <c r="P39" s="1">
         <f t="shared" si="3"/>
@@ -1961,7 +2047,7 @@
     </row>
     <row r="40" spans="1:16" ht="17">
       <c r="B40" s="2" t="s">
-        <v>56</v>
+        <v>85</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>22</v>
@@ -1976,7 +2062,7 @@
       </c>
       <c r="O40" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-500</v>
       </c>
       <c r="P40" s="1">
         <f t="shared" si="3"/>
@@ -1985,7 +2071,7 @@
     </row>
     <row r="41" spans="1:16" ht="34">
       <c r="B41" s="2" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>22</v>
@@ -2003,7 +2089,7 @@
       </c>
       <c r="O41" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-500</v>
       </c>
       <c r="P41" s="1">
         <f t="shared" si="3"/>
@@ -2012,7 +2098,7 @@
     </row>
     <row r="42" spans="1:16" ht="34">
       <c r="B42" s="2" t="s">
-        <v>72</v>
+        <v>87</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>22</v>
@@ -2027,7 +2113,7 @@
       </c>
       <c r="O42" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-500</v>
       </c>
       <c r="P42" s="1">
         <f t="shared" si="3"/>
@@ -2039,7 +2125,7 @@
         <v>1</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>2</v>
@@ -2047,13 +2133,13 @@
       <c r="D43" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G43" s="1" t="s">
+      <c r="G43" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H43" s="1">
-        <v>0</v>
-      </c>
-      <c r="I43" s="1" t="s">
+      <c r="H43" s="4">
+        <v>-500</v>
+      </c>
+      <c r="I43" s="4" t="s">
         <v>2</v>
       </c>
       <c r="M43" s="1" t="str">
@@ -2066,7 +2152,7 @@
       </c>
       <c r="O43" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-500</v>
       </c>
       <c r="P43" s="1">
         <f t="shared" si="3"/>
@@ -2075,14 +2161,14 @@
     </row>
     <row r="44" spans="1:16" ht="34">
       <c r="B44" s="2" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I44" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="G44" s="4"/>
+      <c r="H44" s="4"/>
+      <c r="I44" s="4"/>
       <c r="M44" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Bridge-Connect</v>
@@ -2093,7 +2179,7 @@
       </c>
       <c r="O44" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-500</v>
       </c>
       <c r="P44" s="1">
         <f t="shared" si="3"/>
@@ -2105,7 +2191,7 @@
         <v>0</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>75</v>
+        <v>48</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>24</v>
@@ -2113,10 +2199,11 @@
       <c r="D45" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G45" s="1" t="s">
+      <c r="G45" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="I45" s="1" t="s">
+      <c r="H45" s="4"/>
+      <c r="I45" s="4" t="s">
         <v>2</v>
       </c>
       <c r="M45" s="1" t="str">
@@ -2129,7 +2216,7 @@
       </c>
       <c r="O45" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-500</v>
       </c>
       <c r="P45" s="1">
         <f t="shared" si="3"/>
@@ -2141,7 +2228,7 @@
         <v>1</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>76</v>
+        <v>49</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>2</v>
@@ -2159,7 +2246,7 @@
       </c>
       <c r="O46" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-500</v>
       </c>
       <c r="P46" s="1">
         <f t="shared" si="3"/>
@@ -2171,16 +2258,16 @@
         <v>21</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>79</v>
+        <v>52</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>80</v>
+        <v>53</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>77</v>
+        <v>50</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>71</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
5.31 Enhance Buttons Interaction
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/StoryScript.xlsx
+++ b/Assets/StreamingAssets/StoryScript.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/renqi/TextAdvancedGame/Assets/StreamingAssets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3659303-0708-224F-867B-298B33F90135}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5F50FF1-5A21-7E4C-8568-E1EE225C0EA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1300" windowWidth="28800" windowHeight="16080" xr2:uid="{4FF494A4-B03B-D144-A30E-F081D1418406}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15980" xr2:uid="{4FF494A4-B03B-D144-A30E-F081D1418406}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="91">
   <si>
     <t>Yao</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -390,6 +390,14 @@
   </si>
   <si>
     <t xml:space="preserve"> &lt;color=#00CC00&gt;(I followed Master’s finger, and only then did I spot the faint outline of the manor walls, barely visible in the distant mist.)&lt;/color&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mask</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MaskAction</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -798,10 +806,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40E189AB-F231-6C46-8064-720ADE40C742}">
-  <dimension ref="A1:R47"/>
+  <dimension ref="A1:T48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="U7" sqref="U7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -821,10 +829,12 @@
     <col min="13" max="13" width="18.33203125" style="1" customWidth="1"/>
     <col min="14" max="17" width="10.83203125" style="1"/>
     <col min="18" max="18" width="16.33203125" style="1" customWidth="1"/>
-    <col min="19" max="16384" width="10.83203125" style="1"/>
+    <col min="19" max="19" width="10.83203125" style="1"/>
+    <col min="20" max="20" width="12.1640625" style="1" customWidth="1"/>
+    <col min="21" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="17">
+    <row r="1" spans="1:20" ht="17">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -879,8 +889,14 @@
       <c r="R1" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" ht="17">
+      <c r="S1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="17">
       <c r="B2" s="2" t="s">
         <v>61</v>
       </c>
@@ -894,7 +910,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="34">
+    <row r="3" spans="1:20" ht="34">
       <c r="B3" s="2" t="s">
         <v>62</v>
       </c>
@@ -918,7 +934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="34">
+    <row r="4" spans="1:20" ht="34">
       <c r="B4" s="2" t="s">
         <v>63</v>
       </c>
@@ -942,7 +958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="17">
+    <row r="5" spans="1:20" ht="17">
       <c r="B5" s="2" t="s">
         <v>64</v>
       </c>
@@ -966,7 +982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="17">
+    <row r="6" spans="1:20" ht="17">
       <c r="B6" s="2" t="s">
         <v>65</v>
       </c>
@@ -990,7 +1006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="34">
+    <row r="7" spans="1:20" ht="34">
       <c r="B7" s="2" t="s">
         <v>66</v>
       </c>
@@ -1014,7 +1030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="17">
+    <row r="8" spans="1:20" ht="17">
       <c r="B8" s="2" t="s">
         <v>67</v>
       </c>
@@ -1038,7 +1054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="34">
+    <row r="9" spans="1:20" ht="34">
       <c r="B9" s="2" t="s">
         <v>68</v>
       </c>
@@ -1062,7 +1078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="34">
+    <row r="10" spans="1:20" ht="34">
       <c r="B10" s="2" t="s">
         <v>69</v>
       </c>
@@ -1092,7 +1108,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="17">
+    <row r="11" spans="1:20" ht="17">
       <c r="A11" s="2" t="s">
         <v>0</v>
       </c>
@@ -1131,7 +1147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="34">
+    <row r="12" spans="1:20" ht="34">
       <c r="B12" s="2" t="s">
         <v>70</v>
       </c>
@@ -1158,7 +1174,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="17">
+    <row r="13" spans="1:20" ht="17">
       <c r="A13" s="2" t="s">
         <v>0</v>
       </c>
@@ -1191,7 +1207,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="17">
+    <row r="14" spans="1:20" ht="17">
       <c r="B14" s="2" t="s">
         <v>71</v>
       </c>
@@ -1226,7 +1242,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="17">
+    <row r="15" spans="1:20" ht="17">
       <c r="A15" s="2" t="s">
         <v>1</v>
       </c>
@@ -1265,7 +1281,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="17">
+    <row r="16" spans="1:20" ht="17">
       <c r="A16" s="2" t="s">
         <v>0</v>
       </c>
@@ -2263,10 +2279,12 @@
       <c r="C47" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D47" s="1" t="s">
+    </row>
+    <row r="48" spans="1:16" ht="17">
+      <c r="B48" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E47" s="1" t="s">
+      <c r="C48" s="1" t="s">
         <v>46</v>
       </c>
     </row>

</xml_diff>